<commit_message>
started migrating spaghetti into classes
</commit_message>
<xml_diff>
--- a/Light Synth Arduino pinout.xlsx
+++ b/Light Synth Arduino pinout.xlsx
@@ -1,25 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="27011"/>
-  <workbookPr/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/pete/Projects/Personal/light-synthesiser/"/>
-    </mc:Choice>
-  </mc:AlternateContent>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="6" rupBuild="4505"/>
+  <workbookPr autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="4680" yWindow="1500" windowWidth="28800" windowHeight="17600" tabRatio="500"/>
+    <workbookView xWindow="1900" yWindow="-420" windowWidth="24800" windowHeight="16640" tabRatio="500" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="150000" concurrentCalc="0"/>
+  <calcPr calcId="130407" concurrentCalc="0"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
       <x14:workbookPr defaultImageDpi="32767"/>
     </ext>
-    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="http://schemas.microsoft.com/office/mac/excel/2008/main">
       <mx:ArchID Flags="2"/>
     </ext>
   </extLst>
@@ -27,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="65" uniqueCount="46">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="71" uniqueCount="52">
   <si>
     <t>IOREF</t>
   </si>
@@ -165,13 +161,37 @@
   </si>
   <si>
     <t>ARDUINO UNO Rev3</t>
+  </si>
+  <si>
+    <t>Pulse Duration</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Clock Period</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Timer 1 Prescaler</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Timer 1 Period</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Pulse length</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Timer 1 Comparator (actual value is x - 1)</t>
+    <phoneticPr fontId="2" type="noConversion"/>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="2" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <fonts count="3">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -185,6 +205,10 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="8"/>
+      <name val="Verdana"/>
     </font>
   </fonts>
   <fills count="2">
@@ -336,7 +360,7 @@
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
-  <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleMedium7"/>
+  <tableStyles count="0" defaultTableStyle="TableStyleMedium9"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
@@ -388,7 +412,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
+        <a:latin typeface="Calibri Light"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="Yu Gothic Light"/>
@@ -423,7 +447,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="Yu Gothic"/>
@@ -600,21 +624,21 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" mc:Ignorable="mv" mc:PreserveAttributes="mv:*">
   <dimension ref="A2:H28"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="H30" sqref="H30"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="39" customWidth="1"/>
     <col min="2" max="2" width="2.83203125" customWidth="1"/>
@@ -625,8 +649,8 @@
     <col min="8" max="8" width="22.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:8" ht="17" thickBot="1" x14ac:dyDescent="0.25"/>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:8" ht="16" thickBot="1"/>
+    <row r="3" spans="1:8">
       <c r="B3" s="3"/>
       <c r="C3" s="4"/>
       <c r="D3" s="4"/>
@@ -634,7 +658,7 @@
       <c r="F3" s="4"/>
       <c r="G3" s="5"/>
     </row>
-    <row r="4" spans="1:8" ht="26" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:8" ht="25">
       <c r="B4" s="6"/>
       <c r="C4" s="14" t="s">
         <v>45</v>
@@ -649,7 +673,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:8">
       <c r="B5" s="6"/>
       <c r="C5" s="7"/>
       <c r="D5" s="7"/>
@@ -662,7 +686,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:8">
       <c r="B6" s="6"/>
       <c r="C6" s="7"/>
       <c r="D6" s="7"/>
@@ -675,7 +699,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:8">
       <c r="B7" s="6"/>
       <c r="C7" s="7"/>
       <c r="D7" s="7"/>
@@ -688,7 +712,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:8">
       <c r="B8" s="6"/>
       <c r="C8" s="7"/>
       <c r="D8" s="7"/>
@@ -701,7 +725,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:8">
       <c r="A9" t="s">
         <v>30</v>
       </c>
@@ -719,7 +743,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:8">
       <c r="A10" t="s">
         <v>29</v>
       </c>
@@ -737,7 +761,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:8">
       <c r="A11" t="s">
         <v>30</v>
       </c>
@@ -755,7 +779,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:8">
       <c r="A12" t="s">
         <v>30</v>
       </c>
@@ -773,7 +797,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:8">
       <c r="A13" t="s">
         <v>4</v>
       </c>
@@ -791,7 +815,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:8">
       <c r="A14" t="s">
         <v>4</v>
       </c>
@@ -805,7 +829,7 @@
       <c r="G14" s="8"/>
       <c r="H14" s="13"/>
     </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:8">
       <c r="A15" s="12" t="s">
         <v>31</v>
       </c>
@@ -823,7 +847,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:8">
       <c r="B16" s="6"/>
       <c r="C16" s="2"/>
       <c r="D16" s="7"/>
@@ -836,7 +860,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="17" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:8">
       <c r="A17" t="s">
         <v>32</v>
       </c>
@@ -854,7 +878,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="18" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:8">
       <c r="A18" t="s">
         <v>34</v>
       </c>
@@ -872,7 +896,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="19" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:8">
       <c r="A19" t="s">
         <v>35</v>
       </c>
@@ -890,7 +914,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="20" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:8">
       <c r="A20" t="s">
         <v>36</v>
       </c>
@@ -908,7 +932,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="21" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:8">
       <c r="A21" t="s">
         <v>33</v>
       </c>
@@ -926,7 +950,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="22" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:8">
       <c r="A22" t="s">
         <v>37</v>
       </c>
@@ -944,7 +968,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="23" spans="1:8" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:8" ht="16" thickBot="1">
       <c r="B23" s="9"/>
       <c r="C23" s="10"/>
       <c r="D23" s="10"/>
@@ -952,17 +976,466 @@
       <c r="F23" s="10"/>
       <c r="G23" s="11"/>
     </row>
-    <row r="27" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:8">
       <c r="A27" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="28" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:8">
       <c r="A28" t="s">
         <v>44</v>
       </c>
     </row>
   </sheetData>
+  <sheetCalcPr fullCalcOnLoad="1"/>
+  <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="http://schemas.microsoft.com/office/mac/excel/2008/main">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" mc:Ignorable="mv" mc:PreserveAttributes="mv:*">
+  <dimension ref="A1:E28"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A6" sqref="A6:XFD9"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
+  <cols>
+    <col min="1" max="1" width="35.33203125" customWidth="1"/>
+    <col min="2" max="2" width="24.83203125" customWidth="1"/>
+    <col min="3" max="3" width="27.33203125" customWidth="1"/>
+    <col min="4" max="4" width="16" customWidth="1"/>
+    <col min="5" max="5" width="11.1640625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5">
+      <c r="A1" t="s">
+        <v>47</v>
+      </c>
+      <c r="B1">
+        <f>1/16000000</f>
+        <v>6.2499999999999997E-8</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5">
+      <c r="A5" t="s">
+        <v>46</v>
+      </c>
+      <c r="B5" t="s">
+        <v>48</v>
+      </c>
+      <c r="C5" t="s">
+        <v>51</v>
+      </c>
+      <c r="D5" t="s">
+        <v>49</v>
+      </c>
+      <c r="E5" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5">
+      <c r="A6">
+        <v>1</v>
+      </c>
+      <c r="B6">
+        <v>1</v>
+      </c>
+      <c r="C6">
+        <v>2</v>
+      </c>
+      <c r="D6">
+        <f>2 * $B$1*B6 *C6</f>
+        <v>2.4999999999999999E-7</v>
+      </c>
+      <c r="E6">
+        <f>A6 *D6</f>
+        <v>2.4999999999999999E-7</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5">
+      <c r="A7">
+        <v>255</v>
+      </c>
+      <c r="B7">
+        <v>1</v>
+      </c>
+      <c r="C7">
+        <v>2</v>
+      </c>
+      <c r="D7">
+        <f>2 * $B$1*B7 *C7</f>
+        <v>2.4999999999999999E-7</v>
+      </c>
+      <c r="E7">
+        <f t="shared" ref="E7:E23" si="0">A7 *D7</f>
+        <v>6.3749999999999991E-5</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5">
+      <c r="A8">
+        <v>1</v>
+      </c>
+      <c r="B8">
+        <v>1</v>
+      </c>
+      <c r="C8">
+        <v>65536</v>
+      </c>
+      <c r="D8">
+        <f>2 * $B$1*B8 *C8</f>
+        <v>8.1919999999999996E-3</v>
+      </c>
+      <c r="E8">
+        <f t="shared" si="0"/>
+        <v>8.1919999999999996E-3</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5">
+      <c r="A9">
+        <v>255</v>
+      </c>
+      <c r="B9">
+        <v>1</v>
+      </c>
+      <c r="C9">
+        <v>65536</v>
+      </c>
+      <c r="D9">
+        <f>2 * $B$1*B9 *C9</f>
+        <v>8.1919999999999996E-3</v>
+      </c>
+      <c r="E9">
+        <f t="shared" si="0"/>
+        <v>2.0889599999999997</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5">
+      <c r="A10">
+        <v>1</v>
+      </c>
+      <c r="B10">
+        <v>8</v>
+      </c>
+      <c r="C10">
+        <v>2</v>
+      </c>
+      <c r="D10">
+        <f>2 * $B$1*B10 *C10</f>
+        <v>1.9999999999999999E-6</v>
+      </c>
+      <c r="E10">
+        <f t="shared" si="0"/>
+        <v>1.9999999999999999E-6</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5">
+      <c r="A11">
+        <v>255</v>
+      </c>
+      <c r="B11">
+        <v>8</v>
+      </c>
+      <c r="C11">
+        <v>2</v>
+      </c>
+      <c r="D11">
+        <f>2 * $B$1*B11 *C11</f>
+        <v>1.9999999999999999E-6</v>
+      </c>
+      <c r="E11">
+        <f t="shared" si="0"/>
+        <v>5.0999999999999993E-4</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5">
+      <c r="A12">
+        <v>1</v>
+      </c>
+      <c r="B12">
+        <v>8</v>
+      </c>
+      <c r="C12">
+        <v>65536</v>
+      </c>
+      <c r="D12">
+        <f>2 * $B$1*B12 *C12</f>
+        <v>6.5535999999999997E-2</v>
+      </c>
+      <c r="E12">
+        <f t="shared" ref="E12:E13" si="1">A12 *D12</f>
+        <v>6.5535999999999997E-2</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5">
+      <c r="A13">
+        <v>255</v>
+      </c>
+      <c r="B13">
+        <v>8</v>
+      </c>
+      <c r="C13">
+        <v>65536</v>
+      </c>
+      <c r="D13">
+        <f>2 * $B$1*B13 *C13</f>
+        <v>6.5535999999999997E-2</v>
+      </c>
+      <c r="E13">
+        <f t="shared" si="1"/>
+        <v>16.711679999999998</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5">
+      <c r="A14">
+        <v>1</v>
+      </c>
+      <c r="B14">
+        <v>64</v>
+      </c>
+      <c r="C14">
+        <v>2</v>
+      </c>
+      <c r="D14">
+        <f>2 * $B$1*B14 *C14</f>
+        <v>1.5999999999999999E-5</v>
+      </c>
+      <c r="E14">
+        <f t="shared" si="0"/>
+        <v>1.5999999999999999E-5</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5">
+      <c r="A15">
+        <v>255</v>
+      </c>
+      <c r="B15">
+        <v>64</v>
+      </c>
+      <c r="C15">
+        <v>2</v>
+      </c>
+      <c r="D15">
+        <f>2 * $B$1*B15 *C15</f>
+        <v>1.5999999999999999E-5</v>
+      </c>
+      <c r="E15">
+        <f t="shared" si="0"/>
+        <v>4.0799999999999994E-3</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5">
+      <c r="A16">
+        <v>1</v>
+      </c>
+      <c r="B16">
+        <v>64</v>
+      </c>
+      <c r="C16">
+        <v>65536</v>
+      </c>
+      <c r="D16">
+        <f>2 * $B$1*B16 *C16</f>
+        <v>0.52428799999999998</v>
+      </c>
+      <c r="E16">
+        <f t="shared" ref="E16:E19" si="2">A16 *D16</f>
+        <v>0.52428799999999998</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5">
+      <c r="A17">
+        <v>255</v>
+      </c>
+      <c r="B17">
+        <v>64</v>
+      </c>
+      <c r="C17">
+        <v>65536</v>
+      </c>
+      <c r="D17">
+        <f>2 * $B$1*B17 *C17</f>
+        <v>0.52428799999999998</v>
+      </c>
+      <c r="E17">
+        <f t="shared" si="2"/>
+        <v>133.69343999999998</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5">
+      <c r="A18">
+        <v>1</v>
+      </c>
+      <c r="B18">
+        <v>256</v>
+      </c>
+      <c r="C18">
+        <v>2</v>
+      </c>
+      <c r="D18">
+        <f>2 * $B$1*B18 *C18</f>
+        <v>6.3999999999999997E-5</v>
+      </c>
+      <c r="E18">
+        <f t="shared" si="2"/>
+        <v>6.3999999999999997E-5</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5">
+      <c r="A19">
+        <v>255</v>
+      </c>
+      <c r="B19">
+        <v>256</v>
+      </c>
+      <c r="C19">
+        <v>2</v>
+      </c>
+      <c r="D19">
+        <f>2 * $B$1*B19 *C19</f>
+        <v>6.3999999999999997E-5</v>
+      </c>
+      <c r="E19">
+        <f t="shared" si="2"/>
+        <v>1.6319999999999998E-2</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5">
+      <c r="A20">
+        <v>1</v>
+      </c>
+      <c r="B20">
+        <v>256</v>
+      </c>
+      <c r="C20">
+        <v>65536</v>
+      </c>
+      <c r="D20">
+        <f>2 * $B$1*B20 *C20</f>
+        <v>2.0971519999999999</v>
+      </c>
+      <c r="E20">
+        <f t="shared" si="0"/>
+        <v>2.0971519999999999</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5">
+      <c r="A21">
+        <v>255</v>
+      </c>
+      <c r="B21">
+        <v>256</v>
+      </c>
+      <c r="C21">
+        <v>65536</v>
+      </c>
+      <c r="D21">
+        <f>2 * $B$1*B21 *C21</f>
+        <v>2.0971519999999999</v>
+      </c>
+      <c r="E21">
+        <f t="shared" si="0"/>
+        <v>534.77375999999992</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5" ht="16" customHeight="1">
+      <c r="A22">
+        <v>1</v>
+      </c>
+      <c r="B22">
+        <v>1024</v>
+      </c>
+      <c r="C22">
+        <v>2</v>
+      </c>
+      <c r="D22">
+        <f>2 * $B$1*B22 *C22</f>
+        <v>2.5599999999999999E-4</v>
+      </c>
+      <c r="E22">
+        <f t="shared" si="0"/>
+        <v>2.5599999999999999E-4</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5" ht="16" customHeight="1">
+      <c r="A23">
+        <v>255</v>
+      </c>
+      <c r="B23">
+        <v>1024</v>
+      </c>
+      <c r="C23">
+        <v>2</v>
+      </c>
+      <c r="D23">
+        <f>2 * $B$1*B23 *C23</f>
+        <v>2.5599999999999999E-4</v>
+      </c>
+      <c r="E23">
+        <f t="shared" si="0"/>
+        <v>6.5279999999999991E-2</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5" ht="16" customHeight="1">
+      <c r="A24">
+        <v>1</v>
+      </c>
+      <c r="B24">
+        <v>1024</v>
+      </c>
+      <c r="C24">
+        <v>65536</v>
+      </c>
+      <c r="D24">
+        <f>2 * $B$1*B24 *C24</f>
+        <v>8.3886079999999996</v>
+      </c>
+      <c r="E24">
+        <f t="shared" ref="E24:E25" si="3">A24 *D24</f>
+        <v>8.3886079999999996</v>
+      </c>
+    </row>
+    <row r="25" spans="1:5" ht="16" customHeight="1">
+      <c r="A25">
+        <v>255</v>
+      </c>
+      <c r="B25">
+        <v>1024</v>
+      </c>
+      <c r="C25">
+        <v>65536</v>
+      </c>
+      <c r="D25">
+        <f>2 * $B$1*B25 *C25</f>
+        <v>8.3886079999999996</v>
+      </c>
+      <c r="E25">
+        <f t="shared" si="3"/>
+        <v>2139.0950399999997</v>
+      </c>
+    </row>
+    <row r="28" spans="1:5">
+      <c r="C28">
+        <f>2^16</f>
+        <v>65536</v>
+      </c>
+    </row>
+  </sheetData>
+  <sheetCalcPr fullCalcOnLoad="1"/>
+  <phoneticPr fontId="2" type="noConversion"/>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageSetup paperSize="0" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="http://schemas.microsoft.com/office/mac/excel/2008/main">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
first test with real hardware
</commit_message>
<xml_diff>
--- a/Light Synth Arduino pinout.xlsx
+++ b/Light Synth Arduino pinout.xlsx
@@ -1,15 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="16925"/>
-  <workbookPr/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Users\Pete\My Documents\Projects\light-synthesiser\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="6" rupBuild="4505"/>
+  <workbookPr autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="4680" yWindow="1500" windowWidth="28800" windowHeight="17595" tabRatio="500"/>
+    <workbookView xWindow="-20" yWindow="-20" windowWidth="24800" windowHeight="16640" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -19,7 +14,7 @@
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
       <x14:workbookPr defaultImageDpi="32767"/>
     </ext>
-    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="http://schemas.microsoft.com/office/mac/excel/2008/main">
       <mx:ArchID Flags="2"/>
     </ext>
   </extLst>
@@ -176,8 +171,8 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="2" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <fonts count="3">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -191,6 +186,10 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="8"/>
+      <name val="Verdana"/>
     </font>
   </fonts>
   <fills count="2">
@@ -342,7 +341,7 @@
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
-  <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleMedium7"/>
+  <tableStyles count="0" defaultTableStyle="TableStyleMedium9"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
@@ -397,7 +396,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
+        <a:latin typeface="Calibri Light"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="Yu Gothic Light"/>
@@ -432,7 +431,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="Yu Gothic"/>
@@ -609,34 +608,34 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" mc:Ignorable="mv" mc:PreserveAttributes="mv:*">
   <dimension ref="A2:I28"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K22" sqref="K22"/>
+      <selection activeCell="J22" sqref="J22"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="39" customWidth="1"/>
-    <col min="2" max="2" width="2.875" customWidth="1"/>
-    <col min="3" max="3" width="6.625" customWidth="1"/>
-    <col min="5" max="5" width="16.375" customWidth="1"/>
-    <col min="6" max="6" width="7.125" customWidth="1"/>
-    <col min="7" max="7" width="3.375" customWidth="1"/>
+    <col min="2" max="2" width="2.83203125" customWidth="1"/>
+    <col min="3" max="3" width="6.6640625" customWidth="1"/>
+    <col min="5" max="5" width="16.33203125" customWidth="1"/>
+    <col min="6" max="6" width="7.1640625" customWidth="1"/>
+    <col min="7" max="7" width="3.33203125" customWidth="1"/>
     <col min="8" max="8" width="22.5" customWidth="1"/>
     <col min="9" max="9" width="13.5" style="13" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:9" ht="16.5" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:9" ht="16" thickBot="1"/>
+    <row r="3" spans="1:9">
       <c r="B3" s="3"/>
       <c r="C3" s="4"/>
       <c r="D3" s="4"/>
@@ -644,7 +643,7 @@
       <c r="F3" s="4"/>
       <c r="G3" s="5"/>
     </row>
-    <row r="4" spans="1:9" ht="26.25" x14ac:dyDescent="0.4">
+    <row r="4" spans="1:9" ht="25">
       <c r="B4" s="6"/>
       <c r="C4" s="14" t="s">
         <v>45</v>
@@ -659,7 +658,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:9">
       <c r="B5" s="6"/>
       <c r="C5" s="7"/>
       <c r="D5" s="7"/>
@@ -672,7 +671,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:9">
       <c r="B6" s="6"/>
       <c r="C6" s="7"/>
       <c r="D6" s="7"/>
@@ -685,7 +684,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:9">
       <c r="B7" s="6"/>
       <c r="C7" s="7"/>
       <c r="D7" s="7"/>
@@ -698,7 +697,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:9">
       <c r="B8" s="6"/>
       <c r="C8" s="7"/>
       <c r="D8" s="7"/>
@@ -711,7 +710,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:9">
       <c r="A9" t="s">
         <v>30</v>
       </c>
@@ -729,7 +728,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:9">
       <c r="A10" t="s">
         <v>29</v>
       </c>
@@ -750,7 +749,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:9">
       <c r="A11" t="s">
         <v>30</v>
       </c>
@@ -768,7 +767,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:9">
       <c r="A12" t="s">
         <v>30</v>
       </c>
@@ -786,7 +785,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:9">
       <c r="A13" t="s">
         <v>4</v>
       </c>
@@ -804,7 +803,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:9">
       <c r="A14" t="s">
         <v>4</v>
       </c>
@@ -818,7 +817,7 @@
       <c r="G14" s="8"/>
       <c r="H14" s="13"/>
     </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:9">
       <c r="A15" s="12" t="s">
         <v>31</v>
       </c>
@@ -836,7 +835,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:9">
       <c r="B16" s="6"/>
       <c r="C16" s="2"/>
       <c r="D16" s="7"/>
@@ -849,7 +848,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="17" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:9">
       <c r="A17" t="s">
         <v>32</v>
       </c>
@@ -870,7 +869,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="18" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:9">
       <c r="A18" t="s">
         <v>34</v>
       </c>
@@ -887,8 +886,11 @@
       <c r="H18" s="13" t="s">
         <v>38</v>
       </c>
-    </row>
-    <row r="19" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="I18" s="13" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="19" spans="1:9">
       <c r="A19" t="s">
         <v>35</v>
       </c>
@@ -905,8 +907,11 @@
       <c r="H19" s="13" t="s">
         <v>30</v>
       </c>
-    </row>
-    <row r="20" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="I19" s="13" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="20" spans="1:9">
       <c r="A20" t="s">
         <v>36</v>
       </c>
@@ -924,10 +929,10 @@
         <v>30</v>
       </c>
       <c r="I20" s="13" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="21" spans="1:9" x14ac:dyDescent="0.25">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="21" spans="1:9">
       <c r="A21" t="s">
         <v>33</v>
       </c>
@@ -944,11 +949,8 @@
       <c r="H21" s="13" t="s">
         <v>30</v>
       </c>
-      <c r="I21" s="13" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="22" spans="1:9" x14ac:dyDescent="0.25">
+    </row>
+    <row r="22" spans="1:9">
       <c r="A22" t="s">
         <v>37</v>
       </c>
@@ -965,11 +967,8 @@
       <c r="H22" s="13" t="s">
         <v>30</v>
       </c>
-      <c r="I22" s="13" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="23" spans="1:9" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+    </row>
+    <row r="23" spans="1:9" ht="16" thickBot="1">
       <c r="B23" s="9"/>
       <c r="C23" s="10"/>
       <c r="D23" s="10"/>
@@ -977,17 +976,24 @@
       <c r="F23" s="10"/>
       <c r="G23" s="11"/>
     </row>
-    <row r="27" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:9">
       <c r="A27" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="28" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:9">
       <c r="A28" t="s">
         <v>44</v>
       </c>
     </row>
   </sheetData>
+  <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="0" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="http://schemas.microsoft.com/office/mac/excel/2008/main">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
</xml_diff>